<commit_message>
Did printing logic for billitem
</commit_message>
<xml_diff>
--- a/CarpetsApp/excelTemplates/faktura.xlsx
+++ b/CarpetsApp/excelTemplates/faktura.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>RACUN BR.</t>
   </si>
@@ -85,9 +85,6 @@
     <t>SIRINA/cm</t>
   </si>
   <si>
-    <t>komada</t>
-  </si>
-  <si>
     <t>Kolicina metar kv.</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>UKUPNO</t>
   </si>
   <si>
-    <t>N.Sad,  .</t>
-  </si>
-  <si>
     <t xml:space="preserve">SFERA </t>
   </si>
   <si>
@@ -163,7 +157,7 @@
     <t>2017</t>
   </si>
   <si>
-    <t>719-10-17</t>
+    <t>Racun</t>
   </si>
 </sst>
 </file>
@@ -260,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -408,7 +402,97 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -419,39 +503,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -465,38 +520,27 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -510,24 +554,11 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -538,96 +569,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -638,7 +580,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -649,18 +591,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -684,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -696,7 +634,7 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -717,10 +655,10 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -732,13 +670,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -749,54 +687,107 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -804,71 +795,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1312,19 +1249,19 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="J18" sqref="J18:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="0.140625" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
@@ -1333,17 +1270,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="19" t="s">
-        <v>28</v>
+      <c r="B1" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="27">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+        <v>42</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1352,42 +1289,42 @@
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="62"/>
+        <v>27</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="88"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="B4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="H4" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62"/>
+      <c r="B4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="H4" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="65"/>
+        <v>29</v>
+      </c>
+      <c r="H5" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="90"/>
     </row>
     <row r="6" spans="1:13">
       <c r="H6" s="4"/>
@@ -1397,73 +1334,73 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="87">
+      <c r="I7" s="91">
         <v>107570017</v>
       </c>
-      <c r="J7" s="87"/>
+      <c r="J7" s="91"/>
       <c r="K7" s="8"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>107334750</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+        <v>31</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
-      <c r="M12" s="31"/>
+      <c r="M12" s="29"/>
     </row>
     <row r="13" spans="1:13">
       <c r="F13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13" s="31"/>
+      <c r="H13" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="11"/>
@@ -1472,16 +1409,16 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
-      <c r="M14" s="31"/>
+      <c r="M14" s="29"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="59">
+      <c r="G16" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="52">
         <f ca="1">TODAY()</f>
         <v>43040</v>
       </c>
@@ -1489,10 +1426,10 @@
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1500,349 +1437,315 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="85" t="s">
+      <c r="F18" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="96"/>
+      <c r="J18" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="88" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="82"/>
-      <c r="K18" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="79"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="22" t="s">
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="86"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="80"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:13" ht="0.75" customHeight="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="35">
+      <c r="A20" s="39"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="33">
         <f t="shared" ref="F20:F27" si="0">C20*D20/10000</f>
         <v>0</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="98">
+      <c r="G20" s="37"/>
+      <c r="H20" s="73">
         <f>F20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="98"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="43">
-        <f>I20*K20</f>
-        <v>0</v>
-      </c>
-      <c r="M20" s="25">
-        <f>I20+L20</f>
-        <v>0</v>
-      </c>
+      <c r="I20" s="73"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="41">
+        <f>H20*J20</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" spans="1:13" ht="0.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="32">
+      <c r="A21" s="16"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="16">
+      <c r="G21" s="15"/>
+      <c r="H21" s="69">
         <f t="shared" ref="H21:H27" si="1">F21*G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="99">
-        <f t="shared" ref="I21:I27" si="2">F21*G21</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="100"/>
-      <c r="K21" s="49">
-        <f t="shared" ref="K21:K27" si="3">H21+J21</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="47">
-        <f t="shared" ref="L21:L27" si="4">I13*18%</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="25"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="47" t="e">
+        <f>#REF!+I21</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K21" s="45">
+        <f>I13*18%</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="33">
+      <c r="A22" s="16"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="16">
+      <c r="G22" s="15"/>
+      <c r="H22" s="69">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="99">
+      <c r="I22" s="70"/>
+      <c r="J22" s="47" t="e">
+        <f>#REF!+I22</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K22" s="45">
+        <f>I14*18%</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="23"/>
+    </row>
+    <row r="23" spans="1:13" ht="13.5" hidden="1" thickBot="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="70"/>
+      <c r="J23" s="47" t="e">
+        <f>#REF!+I23</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K23" s="45">
+        <f>I15*18%</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" spans="1:13" ht="13.5" hidden="1" thickBot="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="70"/>
+      <c r="J24" s="47" t="e">
+        <f>#REF!+I24</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K24" s="45">
+        <f>I16*18%</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="23"/>
+    </row>
+    <row r="25" spans="1:13" ht="13.5" hidden="1" thickBot="1">
+      <c r="A25" s="16"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="70"/>
+      <c r="J25" s="47" t="e">
+        <f>#REF!+I25</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K25" s="45">
+        <f>I17*18%</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="23"/>
+    </row>
+    <row r="26" spans="1:13" ht="13.5" hidden="1" thickBot="1">
+      <c r="A26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="70"/>
+      <c r="J26" s="47" t="e">
+        <f>#REF!+I26</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K26" s="45" t="e">
+        <f t="shared" ref="K26:K27" si="2">H18*18%</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L26" s="23"/>
+    </row>
+    <row r="27" spans="1:13" hidden="1">
+      <c r="A27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="73"/>
+      <c r="J27" s="47" t="e">
+        <f>#REF!+I27</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K27" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="100"/>
-      <c r="K22" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="47">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="25"/>
-    </row>
-    <row r="23" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="99">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="100"/>
-      <c r="K23" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="47">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="25"/>
-    </row>
-    <row r="24" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="99">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="100"/>
-      <c r="K24" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="47">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="25"/>
-    </row>
-    <row r="25" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="99">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="100"/>
-      <c r="K25" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="47">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="25"/>
-    </row>
-    <row r="26" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="99">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="100"/>
-      <c r="K26" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="47" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M26" s="25"/>
-    </row>
-    <row r="27" spans="1:13" hidden="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="97">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="98"/>
-      <c r="K27" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="43">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="25"/>
+      <c r="L27" s="23"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="71">
+      <c r="A28" s="58">
         <v>1</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="42"/>
-    </row>
-    <row r="29" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="17"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="40"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="62"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="H29" s="67" t="s">
+      <c r="G29" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="68"/>
-      <c r="J29" s="69">
+      <c r="H29" s="55"/>
+      <c r="I29" s="56">
         <v>674.69</v>
       </c>
-      <c r="K29" s="70"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="1:13" ht="13.5" thickBot="1">
-      <c r="B30" s="54"/>
-      <c r="C30" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="57" t="str">
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="63"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="67" t="str">
         <f>H13</f>
-        <v>719-10-17</v>
-      </c>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
+        <v>Racun</v>
+      </c>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="B31" s="17"/>
+      <c r="B31" s="15"/>
       <c r="H31" t="s">
         <v>11</v>
       </c>
@@ -1851,110 +1754,110 @@
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="B32" s="17"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="30"/>
+      <c r="B32" s="15"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="28"/>
     </row>
     <row r="33" spans="2:13">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:13">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K34" s="5"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="17"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="30"/>
+      <c r="B35" s="15"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="28"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="23" t="s">
-        <v>25</v>
+      <c r="B37" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="G37" s="14"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="92"/>
+      <c r="G37" s="13"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I38" s="5"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
+      <c r="I39" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="51"/>
+      <c r="B40" s="49"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="20" t="s">
+      <c r="J40" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="41" spans="2:13" ht="13.5" thickBot="1">
-      <c r="B41" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="93"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-    </row>
-    <row r="42" spans="2:13" ht="13.5" thickBot="1">
-      <c r="M42" s="58"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="M42" s="68"/>
     </row>
     <row r="43" spans="2:13">
       <c r="B43" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="93" t="s">
+      <c r="F43" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
       <c r="J43" s="5"/>
     </row>
     <row r="51" spans="1:11">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="15"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="14"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="G52" s="14"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
+      <c r="G52" s="13"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
     </row>
     <row r="54" spans="1:11">
       <c r="B54" s="5"/>
@@ -1965,56 +1868,57 @@
       <c r="F55" s="11"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="95"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
-      <c r="E58" s="96"/>
-      <c r="F58" s="96"/>
-      <c r="G58" s="96"/>
-      <c r="H58" s="96"/>
-      <c r="I58" s="96"/>
-      <c r="J58" s="96"/>
-      <c r="K58" s="96"/>
+      <c r="A58" s="83"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="84"/>
+      <c r="I58" s="84"/>
+      <c r="J58" s="84"/>
+      <c r="K58" s="84"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="90"/>
-      <c r="B59" s="90"/>
-      <c r="C59" s="90"/>
-      <c r="D59" s="90"/>
-      <c r="E59" s="90"/>
-      <c r="F59" s="90"/>
+      <c r="A59" s="79"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="79"/>
+      <c r="F59" s="79"/>
       <c r="G59" s="5"/>
-      <c r="H59" s="91"/>
-      <c r="I59" s="91"/>
-      <c r="J59" s="91"/>
-      <c r="K59" s="91"/>
+      <c r="H59" s="80"/>
+      <c r="I59" s="80"/>
+      <c r="J59" s="80"/>
+      <c r="K59" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
+  <mergeCells count="26">
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="G18:G19"/>
+    <mergeCell ref="K18:K19"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="H59:K59"/>
     <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B41:C41"/>
     <mergeCell ref="I39:K39"/>
     <mergeCell ref="A58:K58"/>
     <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H18:I19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="F18:F19"/>
   </mergeCells>

</xml_diff>

<commit_message>
Changed bill print to include dispatcher
</commit_message>
<xml_diff>
--- a/CarpetsApp/excelTemplates/faktura.xlsx
+++ b/CarpetsApp/excelTemplates/faktura.xlsx
@@ -268,7 +268,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -517,17 +517,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -553,21 +542,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -624,7 +598,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -637,24 +611,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -664,31 +624,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -710,56 +649,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,9 +682,6 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,54 +691,41 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -856,18 +737,106 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -912,7 +881,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -935,14 +904,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1309,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1331,857 +1300,855 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="14.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="100"/>
     </row>
     <row r="4" spans="1:13" ht="14.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="23" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="26" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="28"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="103"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="31"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="32" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="104">
         <v>107570017</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="35"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="24">
         <v>94</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="23">
         <v>107334750</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="19" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="9"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="38" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="16"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="41" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="29">
         <f ca="1">TODAY()</f>
-        <v>43046</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
+        <v>43049</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="43" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51" t="s">
+      <c r="J18" s="80"/>
+      <c r="K18" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="52"/>
+      <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55" t="s">
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="61"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="0.75" customHeight="1">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="65">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38">
         <f t="shared" ref="F20:F27" si="0">C20*D20/10000</f>
         <v>0</v>
       </c>
-      <c r="G20" s="66"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="68">
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="95">
         <f>F20*G20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="68"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="70">
+      <c r="J20" s="95"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="41">
         <f>I20*K20</f>
         <v>0</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="9">
         <f>I20+L20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="0.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="73">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="67">
+      <c r="G21" s="44"/>
+      <c r="H21" s="40">
         <f t="shared" ref="H21:H27" si="1">F21*G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="96">
         <f t="shared" ref="I21:I27" si="2">F21*G21</f>
         <v>0</v>
       </c>
-      <c r="J21" s="75"/>
-      <c r="K21" s="76">
+      <c r="J21" s="97"/>
+      <c r="K21" s="47">
         <f t="shared" ref="K21:K27" si="3">H21+J21</f>
         <v>0</v>
       </c>
-      <c r="L21" s="77">
+      <c r="L21" s="46">
         <f t="shared" ref="L21:L27" si="4">I13*18%</f>
         <v>0</v>
       </c>
-      <c r="M21" s="6"/>
+      <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="78">
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="67">
+      <c r="G22" s="44"/>
+      <c r="H22" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="75"/>
-      <c r="K22" s="76">
+      <c r="J22" s="97"/>
+      <c r="K22" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L22" s="77">
+      <c r="L22" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M22" s="6"/>
+      <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="78">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="67">
+      <c r="G23" s="44"/>
+      <c r="H23" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I23" s="74">
+      <c r="I23" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="75"/>
-      <c r="K23" s="76">
+      <c r="J23" s="97"/>
+      <c r="K23" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L23" s="77">
+      <c r="L23" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M23" s="6"/>
+      <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A24" s="71"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="78">
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="72"/>
-      <c r="H24" s="67">
+      <c r="G24" s="44"/>
+      <c r="H24" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="74">
+      <c r="I24" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="75"/>
-      <c r="K24" s="76">
+      <c r="J24" s="97"/>
+      <c r="K24" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L24" s="77">
+      <c r="L24" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M24" s="6"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="78">
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="72"/>
-      <c r="H25" s="67">
+      <c r="G25" s="44"/>
+      <c r="H25" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I25" s="74">
+      <c r="I25" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="75"/>
-      <c r="K25" s="76">
+      <c r="J25" s="97"/>
+      <c r="K25" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L25" s="77">
+      <c r="L25" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M25" s="6"/>
+      <c r="M25" s="9"/>
     </row>
     <row r="26" spans="1:13" ht="13.5" hidden="1" thickBot="1">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="78">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="67">
+      <c r="G26" s="44"/>
+      <c r="H26" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="74">
+      <c r="I26" s="96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="75"/>
-      <c r="K26" s="76">
+      <c r="J26" s="97"/>
+      <c r="K26" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L26" s="77" t="e">
+      <c r="L26" s="46" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M26" s="6"/>
+      <c r="M26" s="9"/>
     </row>
     <row r="27" spans="1:13" hidden="1">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="79">
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="72"/>
-      <c r="H27" s="67">
+      <c r="G27" s="44"/>
+      <c r="H27" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27" s="80">
+      <c r="I27" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="68"/>
-      <c r="K27" s="76">
+      <c r="J27" s="95"/>
+      <c r="K27" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L27" s="70">
+      <c r="L27" s="41">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M27" s="6"/>
+      <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="81">
+      <c r="A28" s="50">
         <v>1</v>
       </c>
-      <c r="B28" s="82"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="10"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A29" s="87"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="89" t="s">
+      <c r="A29" s="56"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="10"/>
+      <c r="J29" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="90"/>
-      <c r="J29" s="91">
+      <c r="K29" s="59">
         <v>674.69</v>
       </c>
-      <c r="K29" s="92"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="1"/>
+      <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A30" s="93"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="95" t="s">
+      <c r="A30" s="60"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="96"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="97" t="str">
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64" t="str">
         <f>H13</f>
         <v>719-10-17</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="16"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16" t="s">
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="16"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="100"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="8"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="16"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="10"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="16"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="102"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="8"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="100"/>
-      <c r="L36" s="100"/>
-      <c r="M36" s="7"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="6"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="16"/>
-      <c r="B37" s="103" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="104"/>
-      <c r="J37" s="104"/>
-      <c r="K37" s="104"/>
-      <c r="L37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="10"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="16"/>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="105"/>
-      <c r="K38" s="105"/>
-      <c r="L38" s="16"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="10"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="36" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="106" t="s">
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="16"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="10"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="16"/>
-      <c r="B40" s="107"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="105" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="K40" s="105"/>
-      <c r="L40" s="16"/>
-    </row>
-    <row r="41" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="108" t="s">
+      <c r="K40" s="71"/>
+      <c r="L40" s="10"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="10"/>
+      <c r="B41" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="108"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-    </row>
-    <row r="42" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="11"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="105"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="108" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="108"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
+      <c r="G43" s="90"/>
+      <c r="H43" s="90"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
     </row>
     <row r="51" spans="1:11">
       <c r="B51" s="1"/>
@@ -2205,33 +2172,54 @@
       <c r="F55" s="2"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
+      <c r="A58" s="92"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="93"/>
+      <c r="G58" s="93"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="93"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="93"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
+      <c r="A59" s="87"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="87"/>
+      <c r="D59" s="87"/>
+      <c r="E59" s="87"/>
+      <c r="F59" s="87"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
+      <c r="H59" s="88"/>
+      <c r="I59" s="88"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="H59:K59"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="F43:H43"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="L18:L19"/>
@@ -2239,27 +2227,6 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G18:G19"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="H59:K59"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>